<commit_message>
Change of position of rooms
</commit_message>
<xml_diff>
--- a/Text Adventure Game/Carte.xlsx
+++ b/Text Adventure Game/Carte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lectures\Games Programming\On recommence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DC4641DE-A41D-41DE-A7EF-2C75858042A8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D0FF0C0-A099-4697-9F50-4C01D3EF2D98}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="7056" xr2:uid="{4E2123AC-EAB9-4B7D-A2CC-DB6660A07928}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>.</t>
   </si>
@@ -42,12 +42,6 @@
     <t>Dining_Room</t>
   </si>
   <si>
-    <t>Starting_Room</t>
-  </si>
-  <si>
-    <t>Weight_Room</t>
-  </si>
-  <si>
     <t>Storage_Room</t>
   </si>
   <si>
@@ -63,7 +57,28 @@
     <t xml:space="preserve">Power_Plant </t>
   </si>
   <si>
-    <t>Elevator</t>
+    <t>weight_room</t>
+  </si>
+  <si>
+    <t>Corridor4</t>
+  </si>
+  <si>
+    <t>Corridor3</t>
+  </si>
+  <si>
+    <t>Corridor2</t>
+  </si>
+  <si>
+    <t>Corridor1</t>
+  </si>
+  <si>
+    <t>Elevator(-1)</t>
+  </si>
+  <si>
+    <t>Elevator(-2)</t>
+  </si>
+  <si>
+    <t>Elevator(0)</t>
   </si>
 </sst>
 </file>
@@ -106,13 +121,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051F1A3B-F65F-463C-9A9C-5E6BEB971F49}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -439,29 +451,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
@@ -472,27 +485,30 @@
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3"/>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
@@ -500,56 +516,37 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D11" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Change of position of rooms"
This reverts commit 2c3671e24caa365aa36485eb1ce626ac9d99c28e.
</commit_message>
<xml_diff>
--- a/Text Adventure Game/Carte.xlsx
+++ b/Text Adventure Game/Carte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lectures\Games Programming\On recommence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D0FF0C0-A099-4697-9F50-4C01D3EF2D98}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DC4641DE-A41D-41DE-A7EF-2C75858042A8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="7056" xr2:uid="{4E2123AC-EAB9-4B7D-A2CC-DB6660A07928}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>.</t>
   </si>
@@ -42,6 +42,12 @@
     <t>Dining_Room</t>
   </si>
   <si>
+    <t>Starting_Room</t>
+  </si>
+  <si>
+    <t>Weight_Room</t>
+  </si>
+  <si>
     <t>Storage_Room</t>
   </si>
   <si>
@@ -57,28 +63,7 @@
     <t xml:space="preserve">Power_Plant </t>
   </si>
   <si>
-    <t>weight_room</t>
-  </si>
-  <si>
-    <t>Corridor4</t>
-  </si>
-  <si>
-    <t>Corridor3</t>
-  </si>
-  <si>
-    <t>Corridor2</t>
-  </si>
-  <si>
-    <t>Corridor1</t>
-  </si>
-  <si>
-    <t>Elevator(-1)</t>
-  </si>
-  <si>
-    <t>Elevator(-2)</t>
-  </si>
-  <si>
-    <t>Elevator(0)</t>
+    <t>Elevator</t>
   </si>
 </sst>
 </file>
@@ -121,10 +106,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051F1A3B-F65F-463C-9A9C-5E6BEB971F49}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -451,30 +439,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
@@ -485,30 +472,27 @@
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2"/>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
@@ -516,37 +500,56 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="B9" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>